<commit_message>
GS 4.1-4.7 plus Template edits 4.3/4.4 - 01/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.3 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6654" uniqueCount="1513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6659" uniqueCount="1516">
   <si>
     <t>PS</t>
   </si>
@@ -4588,18 +4588,33 @@
   <si>
     <t>NE</t>
   </si>
+  <si>
+    <t>P[H]</t>
+  </si>
+  <si>
+    <t>JM-74</t>
+  </si>
+  <si>
+    <t>GD-73</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4796,217 +4811,208 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5291,10 +5297,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1846"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1727" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1130" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U1621" sqref="U1621"/>
+      <selection pane="bottomLeft" activeCell="G1127" sqref="G1127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -15591,7 +15597,7 @@
       <c r="D250" s="23"/>
       <c r="E250" s="19"/>
       <c r="F250" s="19"/>
-      <c r="G250" s="64" t="s">
+      <c r="G250" s="63" t="s">
         <v>1501</v>
       </c>
       <c r="H250" s="19"/>
@@ -15631,7 +15637,7 @@
       <c r="D251" s="23"/>
       <c r="E251" s="19"/>
       <c r="F251" s="19"/>
-      <c r="G251" s="64" t="s">
+      <c r="G251" s="63" t="s">
         <v>1501</v>
       </c>
       <c r="H251" s="19"/>
@@ -15671,7 +15677,7 @@
       <c r="D252" s="23"/>
       <c r="E252" s="19"/>
       <c r="F252" s="19"/>
-      <c r="G252" s="64" t="s">
+      <c r="G252" s="63" t="s">
         <v>1501</v>
       </c>
       <c r="H252" s="19"/>
@@ -21596,7 +21602,7 @@
       </c>
     </row>
     <row r="405" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D405" s="67"/>
+      <c r="D405" s="66"/>
       <c r="E405" s="19"/>
       <c r="F405" s="19"/>
       <c r="G405" s="19"/>
@@ -23734,7 +23740,7 @@
     <row r="460" spans="2:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B460" s="36"/>
       <c r="D460" s="23"/>
-      <c r="E460" s="68"/>
+      <c r="E460" s="67"/>
       <c r="F460" s="19"/>
       <c r="G460" s="19"/>
       <c r="H460" s="19"/>
@@ -23772,7 +23778,7 @@
     </row>
     <row r="461" spans="2:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D461" s="23"/>
-      <c r="E461" s="68"/>
+      <c r="E461" s="67"/>
       <c r="F461" s="19"/>
       <c r="G461" s="19"/>
       <c r="H461" s="19"/>
@@ -24231,8 +24237,12 @@
       <c r="P472" s="7"/>
       <c r="Q472" s="7"/>
       <c r="R472" s="7"/>
-      <c r="S472" s="7"/>
-      <c r="T472" s="7"/>
+      <c r="S472" s="7" t="s">
+        <v>1463</v>
+      </c>
+      <c r="T472" s="7" t="s">
+        <v>1513</v>
+      </c>
       <c r="U472" s="7"/>
       <c r="V472" s="44" t="s">
         <v>96</v>
@@ -28515,7 +28525,7 @@
       </c>
     </row>
     <row r="583" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D583" s="66" t="s">
+      <c r="D583" s="65" t="s">
         <v>1509</v>
       </c>
       <c r="E583" s="19"/>
@@ -28991,7 +29001,7 @@
       <c r="V594" s="44"/>
     </row>
     <row r="595" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A595" s="65" t="s">
+      <c r="A595" s="64" t="s">
         <v>1510</v>
       </c>
       <c r="D595" s="23"/>
@@ -29034,7 +29044,7 @@
       </c>
     </row>
     <row r="596" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A596" s="65" t="s">
+      <c r="A596" s="64" t="s">
         <v>1510</v>
       </c>
       <c r="D596" s="23"/>
@@ -30774,7 +30784,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="641" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="641" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D641" s="23"/>
       <c r="E641" s="19"/>
       <c r="F641" s="19"/>
@@ -30812,7 +30822,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="642" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="642" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D642" s="23"/>
       <c r="E642" s="19"/>
       <c r="F642" s="19"/>
@@ -30850,7 +30860,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="643" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="643" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D643" s="23"/>
       <c r="E643" s="19"/>
       <c r="F643" s="19"/>
@@ -30888,7 +30898,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="644" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="644" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D644" s="23"/>
       <c r="E644" s="19"/>
       <c r="F644" s="19"/>
@@ -30926,7 +30936,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="645" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="645" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D645" s="23"/>
       <c r="E645" s="19"/>
       <c r="F645" s="19"/>
@@ -30964,7 +30974,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="646" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="646" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D646" s="23"/>
       <c r="E646" s="19"/>
       <c r="F646" s="19"/>
@@ -31002,7 +31012,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="647" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="647" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D647" s="23"/>
       <c r="E647" s="19"/>
       <c r="F647" s="19"/>
@@ -31044,7 +31054,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="648" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="648" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D648" s="23"/>
       <c r="E648" s="19"/>
       <c r="F648" s="19"/>
@@ -31084,7 +31094,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="649" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="649" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D649" s="23"/>
       <c r="E649" s="19"/>
       <c r="F649" s="19"/>
@@ -31124,12 +31134,13 @@
         <v>298</v>
       </c>
     </row>
-    <row r="650" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="C650" s="69"/>
-      <c r="D650" s="70"/>
-      <c r="E650" s="71"/>
-      <c r="F650" s="71"/>
-      <c r="G650" s="71"/>
+    <row r="650" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="D650" s="23"/>
+      <c r="E650" s="68" t="s">
+        <v>1514</v>
+      </c>
+      <c r="F650" s="19"/>
+      <c r="G650" s="19"/>
       <c r="H650" s="59" t="s">
         <v>1468</v>
       </c>
@@ -31169,7 +31180,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="651" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="651" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D651" s="23"/>
       <c r="E651" s="19"/>
       <c r="F651" s="19"/>
@@ -31209,7 +31220,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="652" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="652" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D652" s="23"/>
       <c r="E652" s="19"/>
       <c r="F652" s="19"/>
@@ -31249,7 +31260,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="653" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="653" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D653" s="23"/>
       <c r="E653" s="19"/>
       <c r="F653" s="19"/>
@@ -31289,7 +31300,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="654" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="654" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D654" s="23"/>
       <c r="E654" s="19"/>
       <c r="F654" s="19"/>
@@ -31327,7 +31338,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="655" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="655" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D655" s="23"/>
       <c r="E655" s="19"/>
       <c r="F655" s="19"/>
@@ -31365,7 +31376,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="656" spans="3:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="656" spans="4:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D656" s="23"/>
       <c r="E656" s="19"/>
       <c r="F656" s="19"/>
@@ -34872,7 +34883,7 @@
       <c r="E750" s="19"/>
       <c r="F750" s="19"/>
       <c r="G750" s="19"/>
-      <c r="H750" s="60" t="s">
+      <c r="H750" s="59" t="s">
         <v>1469</v>
       </c>
       <c r="I750" s="46" t="s">
@@ -34911,7 +34922,7 @@
       <c r="E751" s="19"/>
       <c r="F751" s="19"/>
       <c r="G751" s="19"/>
-      <c r="H751" s="60" t="s">
+      <c r="H751" s="59" t="s">
         <v>1469</v>
       </c>
       <c r="I751" s="46" t="s">
@@ -34950,7 +34961,7 @@
       <c r="E752" s="19"/>
       <c r="F752" s="19"/>
       <c r="G752" s="19"/>
-      <c r="H752" s="60" t="s">
+      <c r="H752" s="59" t="s">
         <v>1469</v>
       </c>
       <c r="I752" s="46" t="s">
@@ -34989,7 +35000,7 @@
       <c r="E753" s="19"/>
       <c r="F753" s="19"/>
       <c r="G753" s="19"/>
-      <c r="H753" s="60" t="s">
+      <c r="H753" s="59" t="s">
         <v>1469</v>
       </c>
       <c r="I753" s="46" t="s">
@@ -35028,7 +35039,7 @@
       <c r="E754" s="19"/>
       <c r="F754" s="19"/>
       <c r="G754" s="19"/>
-      <c r="H754" s="60" t="s">
+      <c r="H754" s="59" t="s">
         <v>1469</v>
       </c>
       <c r="I754" s="46" t="s">
@@ -35067,7 +35078,7 @@
       <c r="E755" s="19"/>
       <c r="F755" s="19"/>
       <c r="G755" s="19"/>
-      <c r="H755" s="60" t="s">
+      <c r="H755" s="59" t="s">
         <v>1469</v>
       </c>
       <c r="I755" s="46" t="s">
@@ -35088,7 +35099,7 @@
         <f t="shared" si="35"/>
         <v>754</v>
       </c>
-      <c r="N755" s="44" t="s">
+      <c r="N755" s="57" t="s">
         <v>409</v>
       </c>
       <c r="O755" s="6"/>
@@ -47436,7 +47447,7 @@
       <c r="E1082" s="19"/>
       <c r="F1082" s="19"/>
       <c r="G1082" s="19"/>
-      <c r="H1082" s="61" t="s">
+      <c r="H1082" s="60" t="s">
         <v>1474</v>
       </c>
       <c r="I1082" s="46" t="s">
@@ -47475,7 +47486,7 @@
       <c r="E1083" s="19"/>
       <c r="F1083" s="19"/>
       <c r="G1083" s="19"/>
-      <c r="H1083" s="61" t="s">
+      <c r="H1083" s="60" t="s">
         <v>1474</v>
       </c>
       <c r="I1083" s="46" t="s">
@@ -47514,7 +47525,7 @@
       <c r="E1084" s="19"/>
       <c r="F1084" s="19"/>
       <c r="G1084" s="19"/>
-      <c r="H1084" s="61" t="s">
+      <c r="H1084" s="60" t="s">
         <v>1474</v>
       </c>
       <c r="I1084" s="46" t="s">
@@ -47553,7 +47564,7 @@
       <c r="E1085" s="19"/>
       <c r="F1085" s="19"/>
       <c r="G1085" s="19"/>
-      <c r="H1085" s="61" t="s">
+      <c r="H1085" s="60" t="s">
         <v>1474</v>
       </c>
       <c r="I1085" s="46" t="s">
@@ -47592,7 +47603,7 @@
       <c r="E1086" s="19"/>
       <c r="F1086" s="19"/>
       <c r="G1086" s="19"/>
-      <c r="H1086" s="61" t="s">
+      <c r="H1086" s="60" t="s">
         <v>1474</v>
       </c>
       <c r="I1086" s="46" t="s">
@@ -49280,7 +49291,9 @@
     <row r="1131" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1131" s="19"/>
       <c r="F1131" s="19"/>
-      <c r="G1131" s="19"/>
+      <c r="G1131" s="68" t="s">
+        <v>1515</v>
+      </c>
       <c r="H1131" s="59" t="s">
         <v>1475</v>
       </c>
@@ -49319,7 +49332,9 @@
     <row r="1132" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1132" s="19"/>
       <c r="F1132" s="19"/>
-      <c r="G1132" s="19"/>
+      <c r="G1132" s="68" t="s">
+        <v>1515</v>
+      </c>
       <c r="H1132" s="59" t="s">
         <v>1475</v>
       </c>
@@ -61438,7 +61453,7 @@
       </c>
     </row>
     <row r="1450" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1450" s="62" t="s">
+      <c r="A1450" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1450" s="19"/>
@@ -61480,7 +61495,7 @@
       </c>
     </row>
     <row r="1451" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1451" s="62" t="s">
+      <c r="A1451" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1451" s="40"/>
@@ -61523,7 +61538,7 @@
       </c>
     </row>
     <row r="1452" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1452" s="62" t="s">
+      <c r="A1452" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1452" s="40"/>
@@ -61566,7 +61581,7 @@
       </c>
     </row>
     <row r="1453" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1453" s="62" t="s">
+      <c r="A1453" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1453" s="40"/>
@@ -61607,7 +61622,7 @@
       </c>
     </row>
     <row r="1454" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1454" s="62" t="s">
+      <c r="A1454" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1454" s="40"/>
@@ -61652,7 +61667,7 @@
       </c>
     </row>
     <row r="1455" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1455" s="62" t="s">
+      <c r="A1455" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1455" s="40"/>
@@ -61695,7 +61710,7 @@
       </c>
     </row>
     <row r="1456" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1456" s="62" t="s">
+      <c r="A1456" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1456" s="40"/>
@@ -61736,7 +61751,7 @@
       </c>
     </row>
     <row r="1457" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1457" s="62" t="s">
+      <c r="A1457" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1457" s="40"/>
@@ -61781,7 +61796,7 @@
       </c>
     </row>
     <row r="1458" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1458" s="62" t="s">
+      <c r="A1458" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1458" s="40"/>
@@ -61822,7 +61837,7 @@
       </c>
     </row>
     <row r="1459" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1459" s="62" t="s">
+      <c r="A1459" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1459" s="40"/>
@@ -61863,7 +61878,7 @@
       </c>
     </row>
     <row r="1460" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1460" s="62" t="s">
+      <c r="A1460" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1460" s="40"/>
@@ -61904,7 +61919,7 @@
       </c>
     </row>
     <row r="1461" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1461" s="62" t="s">
+      <c r="A1461" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1461" s="40"/>
@@ -61947,7 +61962,7 @@
       </c>
     </row>
     <row r="1462" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1462" s="62" t="s">
+      <c r="A1462" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1462" s="40"/>
@@ -61988,7 +62003,7 @@
       </c>
     </row>
     <row r="1463" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1463" s="62" t="s">
+      <c r="A1463" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1463" s="40"/>
@@ -62029,7 +62044,7 @@
       </c>
     </row>
     <row r="1464" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1464" s="62" t="s">
+      <c r="A1464" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1464" s="40"/>
@@ -62070,7 +62085,7 @@
       </c>
     </row>
     <row r="1465" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1465" s="62" t="s">
+      <c r="A1465" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1465" s="40"/>
@@ -62115,7 +62130,7 @@
       </c>
     </row>
     <row r="1466" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1466" s="62" t="s">
+      <c r="A1466" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1466" s="40"/>
@@ -62156,7 +62171,7 @@
       </c>
     </row>
     <row r="1467" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1467" s="62" t="s">
+      <c r="A1467" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1467" s="40"/>
@@ -62197,7 +62212,7 @@
       </c>
     </row>
     <row r="1468" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1468" s="62" t="s">
+      <c r="A1468" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1468" s="40"/>
@@ -62238,7 +62253,7 @@
       </c>
     </row>
     <row r="1469" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1469" s="62" t="s">
+      <c r="A1469" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1469" s="40"/>
@@ -62281,7 +62296,7 @@
       </c>
     </row>
     <row r="1470" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1470" s="62" t="s">
+      <c r="A1470" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1470" s="40"/>
@@ -62322,7 +62337,7 @@
       </c>
     </row>
     <row r="1471" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1471" s="62" t="s">
+      <c r="A1471" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1471" s="40"/>
@@ -62363,7 +62378,7 @@
       </c>
     </row>
     <row r="1472" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1472" s="62" t="s">
+      <c r="A1472" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1472" s="40"/>
@@ -62404,7 +62419,7 @@
       </c>
     </row>
     <row r="1473" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1473" s="62" t="s">
+      <c r="A1473" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1473" s="40"/>
@@ -62447,7 +62462,7 @@
       </c>
     </row>
     <row r="1474" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1474" s="62" t="s">
+      <c r="A1474" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1474" s="40"/>
@@ -62490,7 +62505,7 @@
       </c>
     </row>
     <row r="1475" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1475" s="62" t="s">
+      <c r="A1475" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1475" s="40"/>
@@ -62531,7 +62546,7 @@
       </c>
     </row>
     <row r="1476" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1476" s="62" t="s">
+      <c r="A1476" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1476" s="40"/>
@@ -62572,7 +62587,7 @@
       </c>
     </row>
     <row r="1477" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1477" s="62" t="s">
+      <c r="A1477" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1477" s="40"/>
@@ -62613,7 +62628,7 @@
       </c>
     </row>
     <row r="1478" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1478" s="62" t="s">
+      <c r="A1478" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1478" s="40"/>
@@ -62656,7 +62671,7 @@
       </c>
     </row>
     <row r="1479" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1479" s="62" t="s">
+      <c r="A1479" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1479" s="40"/>
@@ -62697,7 +62712,7 @@
       </c>
     </row>
     <row r="1480" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1480" s="62" t="s">
+      <c r="A1480" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1480" s="40"/>
@@ -62738,7 +62753,7 @@
       </c>
     </row>
     <row r="1481" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1481" s="62" t="s">
+      <c r="A1481" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1481" s="40"/>
@@ -62779,7 +62794,7 @@
       </c>
     </row>
     <row r="1482" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1482" s="62" t="s">
+      <c r="A1482" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1482" s="40"/>
@@ -62820,7 +62835,7 @@
       </c>
     </row>
     <row r="1483" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1483" s="62" t="s">
+      <c r="A1483" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1483" s="40"/>
@@ -62861,7 +62876,7 @@
       </c>
     </row>
     <row r="1484" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1484" s="62" t="s">
+      <c r="A1484" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1484" s="40"/>
@@ -62902,7 +62917,7 @@
       </c>
     </row>
     <row r="1485" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1485" s="62" t="s">
+      <c r="A1485" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1485" s="40"/>
@@ -62942,7 +62957,7 @@
       </c>
     </row>
     <row r="1486" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1486" s="62" t="s">
+      <c r="A1486" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1486" s="40"/>
@@ -62983,7 +62998,7 @@
       </c>
     </row>
     <row r="1487" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1487" s="62" t="s">
+      <c r="A1487" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1487" s="40"/>
@@ -63024,7 +63039,7 @@
       </c>
     </row>
     <row r="1488" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1488" s="62" t="s">
+      <c r="A1488" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1488" s="40"/>
@@ -63065,7 +63080,7 @@
       </c>
     </row>
     <row r="1489" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1489" s="62" t="s">
+      <c r="A1489" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1489" s="40"/>
@@ -63106,7 +63121,7 @@
       <c r="V1489" s="44"/>
     </row>
     <row r="1490" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1490" s="62" t="s">
+      <c r="A1490" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1490" s="40"/>
@@ -63149,7 +63164,7 @@
       </c>
     </row>
     <row r="1491" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1491" s="62" t="s">
+      <c r="A1491" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1491" s="40"/>
@@ -63190,7 +63205,7 @@
       </c>
     </row>
     <row r="1492" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1492" s="62" t="s">
+      <c r="A1492" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1492" s="40"/>
@@ -63231,7 +63246,7 @@
       </c>
     </row>
     <row r="1493" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1493" s="62" t="s">
+      <c r="A1493" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1493" s="40"/>
@@ -63272,7 +63287,7 @@
       </c>
     </row>
     <row r="1494" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1494" s="62" t="s">
+      <c r="A1494" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1494" s="40"/>
@@ -63315,7 +63330,7 @@
       </c>
     </row>
     <row r="1495" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1495" s="62" t="s">
+      <c r="A1495" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1495" s="40"/>
@@ -63358,7 +63373,7 @@
       </c>
     </row>
     <row r="1496" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1496" s="62" t="s">
+      <c r="A1496" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1496" s="40"/>
@@ -63401,7 +63416,7 @@
       </c>
     </row>
     <row r="1497" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1497" s="62" t="s">
+      <c r="A1497" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1497" s="40"/>
@@ -63444,7 +63459,7 @@
       <c r="V1497" s="44"/>
     </row>
     <row r="1498" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1498" s="62" t="s">
+      <c r="A1498" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1498" s="40"/>
@@ -63486,7 +63501,7 @@
       </c>
     </row>
     <row r="1499" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1499" s="62" t="s">
+      <c r="A1499" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1499" s="40"/>
@@ -63529,7 +63544,7 @@
       </c>
     </row>
     <row r="1500" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1500" s="62" t="s">
+      <c r="A1500" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1500" s="40"/>
@@ -63570,7 +63585,7 @@
       </c>
     </row>
     <row r="1501" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1501" s="62" t="s">
+      <c r="A1501" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1501" s="40"/>
@@ -63611,7 +63626,7 @@
       </c>
     </row>
     <row r="1502" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1502" s="62" t="s">
+      <c r="A1502" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1502" s="40"/>
@@ -63652,7 +63667,7 @@
       </c>
     </row>
     <row r="1503" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1503" s="62" t="s">
+      <c r="A1503" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1503" s="40"/>
@@ -63693,7 +63708,7 @@
       </c>
     </row>
     <row r="1504" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1504" s="62" t="s">
+      <c r="A1504" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1504" s="40"/>
@@ -63734,7 +63749,7 @@
       </c>
     </row>
     <row r="1505" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1505" s="62" t="s">
+      <c r="A1505" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1505" s="40"/>
@@ -63775,7 +63790,7 @@
       </c>
     </row>
     <row r="1506" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1506" s="62" t="s">
+      <c r="A1506" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1506" s="40"/>
@@ -63816,7 +63831,7 @@
       </c>
     </row>
     <row r="1507" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1507" s="62" t="s">
+      <c r="A1507" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1507" s="40"/>
@@ -63857,7 +63872,7 @@
       <c r="V1507" s="44"/>
     </row>
     <row r="1508" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1508" s="62" t="s">
+      <c r="A1508" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1508" s="40"/>
@@ -63898,7 +63913,7 @@
       </c>
     </row>
     <row r="1509" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1509" s="62" t="s">
+      <c r="A1509" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1509" s="40"/>
@@ -63941,7 +63956,7 @@
       </c>
     </row>
     <row r="1510" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1510" s="62" t="s">
+      <c r="A1510" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1510" s="40"/>
@@ -63984,7 +63999,7 @@
       </c>
     </row>
     <row r="1511" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1511" s="62" t="s">
+      <c r="A1511" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1511" s="40"/>
@@ -64027,7 +64042,7 @@
       </c>
     </row>
     <row r="1512" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1512" s="62" t="s">
+      <c r="A1512" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1512" s="40"/>
@@ -64070,7 +64085,7 @@
       </c>
     </row>
     <row r="1513" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1513" s="62" t="s">
+      <c r="A1513" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1513" s="40"/>
@@ -64115,7 +64130,7 @@
       </c>
     </row>
     <row r="1514" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1514" s="62" t="s">
+      <c r="A1514" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1514" s="40"/>
@@ -64162,7 +64177,7 @@
       </c>
     </row>
     <row r="1515" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1515" s="62" t="s">
+      <c r="A1515" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1515" s="40"/>
@@ -64203,7 +64218,7 @@
       </c>
     </row>
     <row r="1516" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1516" s="62" t="s">
+      <c r="A1516" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1516" s="40"/>
@@ -64244,7 +64259,7 @@
       </c>
     </row>
     <row r="1517" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1517" s="62" t="s">
+      <c r="A1517" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1517" s="40"/>
@@ -64288,7 +64303,7 @@
       </c>
     </row>
     <row r="1518" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1518" s="62" t="s">
+      <c r="A1518" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1518" s="40"/>
@@ -64331,7 +64346,7 @@
       </c>
     </row>
     <row r="1519" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1519" s="62" t="s">
+      <c r="A1519" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1519" s="40"/>
@@ -64372,7 +64387,7 @@
       </c>
     </row>
     <row r="1520" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1520" s="62" t="s">
+      <c r="A1520" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1520" s="40"/>
@@ -64415,7 +64430,7 @@
       </c>
     </row>
     <row r="1521" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1521" s="62" t="s">
+      <c r="A1521" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1521" s="40"/>
@@ -64456,7 +64471,7 @@
       </c>
     </row>
     <row r="1522" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1522" s="62" t="s">
+      <c r="A1522" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1522" s="40"/>
@@ -64497,7 +64512,7 @@
       </c>
     </row>
     <row r="1523" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1523" s="62" t="s">
+      <c r="A1523" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1523" s="40"/>
@@ -64540,7 +64555,7 @@
       </c>
     </row>
     <row r="1524" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1524" s="62" t="s">
+      <c r="A1524" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1524" s="40"/>
@@ -64583,7 +64598,7 @@
       </c>
     </row>
     <row r="1525" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1525" s="62" t="s">
+      <c r="A1525" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1525" s="40"/>
@@ -64628,7 +64643,7 @@
       </c>
     </row>
     <row r="1526" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1526" s="62" t="s">
+      <c r="A1526" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1526" s="40"/>
@@ -64671,7 +64686,7 @@
       </c>
     </row>
     <row r="1527" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1527" s="62" t="s">
+      <c r="A1527" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1527" s="40"/>
@@ -64714,7 +64729,7 @@
       </c>
     </row>
     <row r="1528" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1528" s="62" t="s">
+      <c r="A1528" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1528" s="40"/>
@@ -64759,7 +64774,7 @@
       </c>
     </row>
     <row r="1529" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1529" s="62" t="s">
+      <c r="A1529" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1529" s="40"/>
@@ -64800,7 +64815,7 @@
       </c>
     </row>
     <row r="1530" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1530" s="62" t="s">
+      <c r="A1530" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1530" s="40"/>
@@ -64841,7 +64856,7 @@
       </c>
     </row>
     <row r="1531" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1531" s="62" t="s">
+      <c r="A1531" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="C1531" s="40"/>
@@ -64882,7 +64897,7 @@
       </c>
     </row>
     <row r="1532" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1532" s="62" t="s">
+      <c r="A1532" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1532" s="19"/>
@@ -64922,7 +64937,7 @@
       </c>
     </row>
     <row r="1533" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1533" s="62" t="s">
+      <c r="A1533" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1533" s="19"/>
@@ -64962,7 +64977,7 @@
       </c>
     </row>
     <row r="1534" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1534" s="62" t="s">
+      <c r="A1534" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1534" s="19"/>
@@ -65004,7 +65019,7 @@
       </c>
     </row>
     <row r="1535" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1535" s="62" t="s">
+      <c r="A1535" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1535" s="19"/>
@@ -65044,7 +65059,7 @@
       </c>
     </row>
     <row r="1536" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1536" s="62" t="s">
+      <c r="A1536" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1536" s="19"/>
@@ -65084,7 +65099,7 @@
       </c>
     </row>
     <row r="1537" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1537" s="62" t="s">
+      <c r="A1537" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1537" s="19"/>
@@ -65126,7 +65141,7 @@
       </c>
     </row>
     <row r="1538" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1538" s="62" t="s">
+      <c r="A1538" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1538" s="19"/>
@@ -65166,7 +65181,7 @@
       </c>
     </row>
     <row r="1539" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1539" s="62" t="s">
+      <c r="A1539" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1539" s="19"/>
@@ -65206,7 +65221,7 @@
       </c>
     </row>
     <row r="1540" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1540" s="62" t="s">
+      <c r="A1540" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1540" s="19"/>
@@ -65248,7 +65263,7 @@
       </c>
     </row>
     <row r="1541" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1541" s="62" t="s">
+      <c r="A1541" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1541" s="19"/>
@@ -65290,7 +65305,7 @@
       </c>
     </row>
     <row r="1542" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1542" s="62" t="s">
+      <c r="A1542" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1542" s="19"/>
@@ -65330,7 +65345,7 @@
       </c>
     </row>
     <row r="1543" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1543" s="62" t="s">
+      <c r="A1543" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1543" s="19"/>
@@ -65370,7 +65385,7 @@
       </c>
     </row>
     <row r="1544" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1544" s="62" t="s">
+      <c r="A1544" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1544" s="19"/>
@@ -65410,7 +65425,7 @@
       </c>
     </row>
     <row r="1545" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1545" s="62" t="s">
+      <c r="A1545" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1545" s="19"/>
@@ -65450,7 +65465,7 @@
       </c>
     </row>
     <row r="1546" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1546" s="62" t="s">
+      <c r="A1546" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1546" s="19"/>
@@ -65492,7 +65507,7 @@
       </c>
     </row>
     <row r="1547" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1547" s="62" t="s">
+      <c r="A1547" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1547" s="19"/>
@@ -65532,7 +65547,7 @@
       </c>
     </row>
     <row r="1548" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1548" s="62" t="s">
+      <c r="A1548" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1548" s="19"/>
@@ -65572,7 +65587,7 @@
       </c>
     </row>
     <row r="1549" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1549" s="62" t="s">
+      <c r="A1549" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1549" s="19"/>
@@ -65612,7 +65627,7 @@
       </c>
     </row>
     <row r="1550" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1550" s="62" t="s">
+      <c r="A1550" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1550" s="19"/>
@@ -65654,7 +65669,7 @@
       </c>
     </row>
     <row r="1551" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1551" s="62" t="s">
+      <c r="A1551" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1551" s="19"/>
@@ -65694,7 +65709,7 @@
       </c>
     </row>
     <row r="1552" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1552" s="62" t="s">
+      <c r="A1552" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1552" s="19"/>
@@ -65736,7 +65751,7 @@
       </c>
     </row>
     <row r="1553" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1553" s="62" t="s">
+      <c r="A1553" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1553" s="19"/>
@@ -65776,7 +65791,7 @@
       </c>
     </row>
     <row r="1554" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1554" s="62" t="s">
+      <c r="A1554" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1554" s="19"/>
@@ -65818,7 +65833,7 @@
       </c>
     </row>
     <row r="1555" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1555" s="62" t="s">
+      <c r="A1555" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1555" s="19"/>
@@ -65860,7 +65875,7 @@
       </c>
     </row>
     <row r="1556" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1556" s="62" t="s">
+      <c r="A1556" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1556" s="19"/>
@@ -65902,7 +65917,7 @@
       </c>
     </row>
     <row r="1557" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1557" s="62" t="s">
+      <c r="A1557" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1557" s="19"/>
@@ -65944,7 +65959,7 @@
       </c>
     </row>
     <row r="1558" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1558" s="62" t="s">
+      <c r="A1558" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1558" s="19"/>
@@ -65986,7 +66001,7 @@
       </c>
     </row>
     <row r="1559" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1559" s="62" t="s">
+      <c r="A1559" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1559" s="19"/>
@@ -66028,7 +66043,7 @@
       </c>
     </row>
     <row r="1560" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1560" s="62" t="s">
+      <c r="A1560" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1560" s="19"/>
@@ -66070,7 +66085,7 @@
       </c>
     </row>
     <row r="1561" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1561" s="62" t="s">
+      <c r="A1561" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1561" s="19"/>
@@ -66110,7 +66125,7 @@
       </c>
     </row>
     <row r="1562" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1562" s="62" t="s">
+      <c r="A1562" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1562" s="19"/>
@@ -66150,7 +66165,7 @@
       </c>
     </row>
     <row r="1563" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1563" s="62" t="s">
+      <c r="A1563" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1563" s="19"/>
@@ -66190,7 +66205,7 @@
       </c>
     </row>
     <row r="1564" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1564" s="62" t="s">
+      <c r="A1564" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1564" s="19"/>
@@ -66232,7 +66247,7 @@
       </c>
     </row>
     <row r="1565" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1565" s="62" t="s">
+      <c r="A1565" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1565" s="19"/>
@@ -66272,7 +66287,7 @@
       </c>
     </row>
     <row r="1566" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1566" s="62" t="s">
+      <c r="A1566" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1566" s="19"/>
@@ -66312,7 +66327,7 @@
       </c>
     </row>
     <row r="1567" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1567" s="62" t="s">
+      <c r="A1567" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1567" s="19"/>
@@ -66354,7 +66369,7 @@
       </c>
     </row>
     <row r="1568" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1568" s="62" t="s">
+      <c r="A1568" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1568" s="18"/>
@@ -66394,7 +66409,7 @@
       </c>
     </row>
     <row r="1569" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1569" s="62" t="s">
+      <c r="A1569" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1569" s="19"/>
@@ -66434,7 +66449,7 @@
       </c>
     </row>
     <row r="1570" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1570" s="62" t="s">
+      <c r="A1570" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1570" s="19"/>
@@ -66476,7 +66491,7 @@
       </c>
     </row>
     <row r="1571" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1571" s="62" t="s">
+      <c r="A1571" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1571" s="19"/>
@@ -66516,7 +66531,7 @@
       </c>
     </row>
     <row r="1572" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1572" s="62" t="s">
+      <c r="A1572" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1572" s="19"/>
@@ -66560,7 +66575,7 @@
       </c>
     </row>
     <row r="1573" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1573" s="62" t="s">
+      <c r="A1573" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1573" s="19"/>
@@ -66600,7 +66615,7 @@
       </c>
     </row>
     <row r="1574" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1574" s="62" t="s">
+      <c r="A1574" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1574" s="19"/>
@@ -66640,7 +66655,7 @@
       </c>
     </row>
     <row r="1575" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1575" s="62" t="s">
+      <c r="A1575" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1575" s="19"/>
@@ -66682,7 +66697,7 @@
       </c>
     </row>
     <row r="1576" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1576" s="62" t="s">
+      <c r="A1576" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1576" s="19"/>
@@ -66722,7 +66737,7 @@
       </c>
     </row>
     <row r="1577" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1577" s="62" t="s">
+      <c r="A1577" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="E1577" s="19"/>
@@ -66762,7 +66777,7 @@
       </c>
     </row>
     <row r="1578" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1578" s="62" t="s">
+      <c r="A1578" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1578" s="46" t="s">
@@ -66798,7 +66813,7 @@
       </c>
     </row>
     <row r="1579" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1579" s="62" t="s">
+      <c r="A1579" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1579" s="46" t="s">
@@ -66838,7 +66853,7 @@
       </c>
     </row>
     <row r="1580" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1580" s="62" t="s">
+      <c r="A1580" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1580" s="46" t="s">
@@ -66874,7 +66889,7 @@
       </c>
     </row>
     <row r="1581" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1581" s="62" t="s">
+      <c r="A1581" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1581" s="46" t="s">
@@ -66903,7 +66918,7 @@
       </c>
     </row>
     <row r="1582" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1582" s="62" t="s">
+      <c r="A1582" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1582" s="46" t="s">
@@ -66935,7 +66950,7 @@
       </c>
     </row>
     <row r="1583" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1583" s="62" t="s">
+      <c r="A1583" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1583" s="46" t="s">
@@ -66967,7 +66982,7 @@
       </c>
     </row>
     <row r="1584" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1584" s="62" t="s">
+      <c r="A1584" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1584" s="46" t="s">
@@ -66996,7 +67011,7 @@
       </c>
     </row>
     <row r="1585" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1585" s="62" t="s">
+      <c r="A1585" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1585" s="46" t="s">
@@ -67025,7 +67040,7 @@
       </c>
     </row>
     <row r="1586" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1586" s="62" t="s">
+      <c r="A1586" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1586" s="46" t="s">
@@ -67054,7 +67069,7 @@
       </c>
     </row>
     <row r="1587" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1587" s="62" t="s">
+      <c r="A1587" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1587" s="46" t="s">
@@ -67083,7 +67098,7 @@
       </c>
     </row>
     <row r="1588" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1588" s="62" t="s">
+      <c r="A1588" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1588" s="46" t="s">
@@ -67115,7 +67130,7 @@
       </c>
     </row>
     <row r="1589" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1589" s="62" t="s">
+      <c r="A1589" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1589" s="59" t="s">
@@ -67147,7 +67162,7 @@
       </c>
     </row>
     <row r="1590" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1590" s="62" t="s">
+      <c r="A1590" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1590" s="59" t="s">
@@ -67179,7 +67194,7 @@
       </c>
     </row>
     <row r="1591" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1591" s="62" t="s">
+      <c r="A1591" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1591" s="59" t="s">
@@ -67217,7 +67232,7 @@
       </c>
     </row>
     <row r="1592" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1592" s="62" t="s">
+      <c r="A1592" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1592" s="46" t="s">
@@ -67246,7 +67261,7 @@
       </c>
     </row>
     <row r="1593" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1593" s="62" t="s">
+      <c r="A1593" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1593" s="46" t="s">
@@ -67275,7 +67290,7 @@
       </c>
     </row>
     <row r="1594" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1594" s="62" t="s">
+      <c r="A1594" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1594" s="46" t="s">
@@ -67304,7 +67319,7 @@
       </c>
     </row>
     <row r="1595" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1595" s="62" t="s">
+      <c r="A1595" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1595" s="46" t="s">
@@ -67333,7 +67348,7 @@
       </c>
     </row>
     <row r="1596" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1596" s="62" t="s">
+      <c r="A1596" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1596" s="46" t="s">
@@ -67365,7 +67380,7 @@
       </c>
     </row>
     <row r="1597" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1597" s="62" t="s">
+      <c r="A1597" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1597" s="46" t="s">
@@ -67394,7 +67409,7 @@
       </c>
     </row>
     <row r="1598" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1598" s="62" t="s">
+      <c r="A1598" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1598" s="46" t="s">
@@ -67423,7 +67438,7 @@
       </c>
     </row>
     <row r="1599" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1599" s="62" t="s">
+      <c r="A1599" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1599" s="46" t="s">
@@ -67452,7 +67467,7 @@
       </c>
     </row>
     <row r="1600" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1600" s="62" t="s">
+      <c r="A1600" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1600" s="46" t="s">
@@ -67484,7 +67499,7 @@
       </c>
     </row>
     <row r="1601" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1601" s="62" t="s">
+      <c r="A1601" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1601" s="46" t="s">
@@ -67513,7 +67528,7 @@
       </c>
     </row>
     <row r="1602" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1602" s="62" t="s">
+      <c r="A1602" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1602" s="46" t="s">
@@ -67542,7 +67557,7 @@
       </c>
     </row>
     <row r="1603" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1603" s="62" t="s">
+      <c r="A1603" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1603" s="46" t="s">
@@ -67572,7 +67587,7 @@
       <c r="V1603" s="44"/>
     </row>
     <row r="1604" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1604" s="62" t="s">
+      <c r="A1604" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1604" s="46" t="s">
@@ -67601,7 +67616,7 @@
       </c>
     </row>
     <row r="1605" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1605" s="62" t="s">
+      <c r="A1605" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1605" s="46" t="s">
@@ -67630,7 +67645,7 @@
       </c>
     </row>
     <row r="1606" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1606" s="62" t="s">
+      <c r="A1606" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1606" s="46" t="s">
@@ -67659,10 +67674,10 @@
       </c>
     </row>
     <row r="1607" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1607" s="62" t="s">
+      <c r="A1607" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="F1607" s="65" t="s">
+      <c r="F1607" s="64" t="s">
         <v>1504</v>
       </c>
       <c r="I1607" s="46" t="s">
@@ -67691,10 +67706,10 @@
       </c>
     </row>
     <row r="1608" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1608" s="62" t="s">
+      <c r="A1608" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="F1608" s="65" t="s">
+      <c r="F1608" s="64" t="s">
         <v>1504</v>
       </c>
       <c r="I1608" s="46" t="s">
@@ -67726,10 +67741,10 @@
       </c>
     </row>
     <row r="1609" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1609" s="62" t="s">
+      <c r="A1609" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="F1609" s="65" t="s">
+      <c r="F1609" s="64" t="s">
         <v>1504</v>
       </c>
       <c r="I1609" s="46" t="s">
@@ -67761,7 +67776,7 @@
       </c>
     </row>
     <row r="1610" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1610" s="62" t="s">
+      <c r="A1610" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1610" s="46" t="s">
@@ -67793,7 +67808,7 @@
       </c>
     </row>
     <row r="1611" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1611" s="62" t="s">
+      <c r="A1611" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1611" s="46" t="s">
@@ -67822,7 +67837,7 @@
       </c>
     </row>
     <row r="1612" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1612" s="62" t="s">
+      <c r="A1612" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1612" s="46" t="s">
@@ -67854,7 +67869,7 @@
       </c>
     </row>
     <row r="1613" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1613" s="62" t="s">
+      <c r="A1613" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1613" s="46" t="s">
@@ -67886,7 +67901,7 @@
       </c>
     </row>
     <row r="1614" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1614" s="62" t="s">
+      <c r="A1614" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1614" s="46" t="s">
@@ -67918,7 +67933,7 @@
       </c>
     </row>
     <row r="1615" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1615" s="62" t="s">
+      <c r="A1615" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1615" s="46" t="s">
@@ -67950,7 +67965,7 @@
       </c>
     </row>
     <row r="1616" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1616" s="62" t="s">
+      <c r="A1616" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1616" s="46" t="s">
@@ -67979,7 +67994,7 @@
       </c>
     </row>
     <row r="1617" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1617" s="62" t="s">
+      <c r="A1617" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1617" s="46" t="s">
@@ -68008,7 +68023,7 @@
       </c>
     </row>
     <row r="1618" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1618" s="62" t="s">
+      <c r="A1618" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1618" s="46" t="s">
@@ -68037,7 +68052,7 @@
       </c>
     </row>
     <row r="1619" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1619" s="62" t="s">
+      <c r="A1619" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1619" s="59" t="s">
@@ -68070,7 +68085,7 @@
       <c r="V1619" s="44"/>
     </row>
     <row r="1620" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1620" s="62" t="s">
+      <c r="A1620" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1620" s="59" t="s">
@@ -68102,7 +68117,7 @@
       </c>
     </row>
     <row r="1621" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1621" s="62" t="s">
+      <c r="A1621" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1621" s="59" t="s">
@@ -68137,7 +68152,7 @@
       </c>
     </row>
     <row r="1622" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1622" s="62" t="s">
+      <c r="A1622" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1622" s="46" t="s">
@@ -68169,7 +68184,7 @@
       </c>
     </row>
     <row r="1623" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1623" s="62" t="s">
+      <c r="A1623" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1623" s="46" t="s">
@@ -68198,7 +68213,7 @@
       </c>
     </row>
     <row r="1624" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1624" s="62" t="s">
+      <c r="A1624" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1624" s="46" t="s">
@@ -68230,7 +68245,7 @@
       </c>
     </row>
     <row r="1625" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1625" s="62" t="s">
+      <c r="A1625" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1625" s="46" t="s">
@@ -68259,7 +68274,7 @@
       </c>
     </row>
     <row r="1626" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1626" s="62" t="s">
+      <c r="A1626" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1626" s="46" t="s">
@@ -68288,7 +68303,7 @@
       </c>
     </row>
     <row r="1627" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1627" s="62" t="s">
+      <c r="A1627" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1627" s="46" t="s">
@@ -68317,7 +68332,7 @@
       </c>
     </row>
     <row r="1628" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1628" s="62" t="s">
+      <c r="A1628" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1628" s="59" t="s">
@@ -68349,7 +68364,7 @@
       </c>
     </row>
     <row r="1629" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1629" s="62" t="s">
+      <c r="A1629" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1629" s="59" t="s">
@@ -68387,13 +68402,13 @@
       </c>
     </row>
     <row r="1630" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1630" s="62" t="s">
+      <c r="A1630" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="D1630" s="66" t="s">
+      <c r="D1630" s="65" t="s">
         <v>1508</v>
       </c>
-      <c r="F1630" s="65" t="s">
+      <c r="F1630" s="64" t="s">
         <v>1507</v>
       </c>
       <c r="H1630" s="59" t="s">
@@ -68431,13 +68446,13 @@
       </c>
     </row>
     <row r="1631" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1631" s="62" t="s">
+      <c r="A1631" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="D1631" s="66" t="s">
+      <c r="D1631" s="65" t="s">
         <v>1508</v>
       </c>
-      <c r="F1631" s="65" t="s">
+      <c r="F1631" s="64" t="s">
         <v>1507</v>
       </c>
       <c r="H1631" s="59" t="s">
@@ -68472,7 +68487,7 @@
       </c>
     </row>
     <row r="1632" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1632" s="62" t="s">
+      <c r="A1632" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1632" s="59" t="s">
@@ -68504,7 +68519,7 @@
       </c>
     </row>
     <row r="1633" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1633" s="62" t="s">
+      <c r="A1633" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1633" s="59" t="s">
@@ -68539,7 +68554,7 @@
       </c>
     </row>
     <row r="1634" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1634" s="62" t="s">
+      <c r="A1634" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1634" s="46" t="s">
@@ -68568,7 +68583,7 @@
       </c>
     </row>
     <row r="1635" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1635" s="62" t="s">
+      <c r="A1635" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1635" s="46" t="s">
@@ -68597,7 +68612,7 @@
       </c>
     </row>
     <row r="1636" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1636" s="62" t="s">
+      <c r="A1636" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1636" s="46" t="s">
@@ -68626,7 +68641,7 @@
       </c>
     </row>
     <row r="1637" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1637" s="62" t="s">
+      <c r="A1637" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1637" s="46" t="s">
@@ -68655,7 +68670,7 @@
       </c>
     </row>
     <row r="1638" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1638" s="62" t="s">
+      <c r="A1638" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1638" s="46" t="s">
@@ -68684,7 +68699,7 @@
       </c>
     </row>
     <row r="1639" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1639" s="62" t="s">
+      <c r="A1639" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1639" s="46" t="s">
@@ -68713,7 +68728,7 @@
       </c>
     </row>
     <row r="1640" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1640" s="62" t="s">
+      <c r="A1640" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1640" s="46" t="s">
@@ -68742,7 +68757,7 @@
       </c>
     </row>
     <row r="1641" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1641" s="62" t="s">
+      <c r="A1641" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1641" s="46" t="s">
@@ -68771,7 +68786,7 @@
       </c>
     </row>
     <row r="1642" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1642" s="62" t="s">
+      <c r="A1642" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1642" s="46" t="s">
@@ -68806,7 +68821,7 @@
       </c>
     </row>
     <row r="1643" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1643" s="62" t="s">
+      <c r="A1643" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1643" s="46" t="s">
@@ -68835,7 +68850,7 @@
       </c>
     </row>
     <row r="1644" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1644" s="62" t="s">
+      <c r="A1644" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1644" s="46" t="s">
@@ -68864,7 +68879,7 @@
       </c>
     </row>
     <row r="1645" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1645" s="62" t="s">
+      <c r="A1645" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1645" s="46" t="s">
@@ -68893,7 +68908,7 @@
       </c>
     </row>
     <row r="1646" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1646" s="62" t="s">
+      <c r="A1646" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1646" s="46" t="s">
@@ -68922,7 +68937,7 @@
       </c>
     </row>
     <row r="1647" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1647" s="62" t="s">
+      <c r="A1647" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1647" s="46" t="s">
@@ -68951,7 +68966,7 @@
       </c>
     </row>
     <row r="1648" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1648" s="62" t="s">
+      <c r="A1648" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1648" s="46" t="s">
@@ -68980,7 +68995,7 @@
       </c>
     </row>
     <row r="1649" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1649" s="62" t="s">
+      <c r="A1649" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1649" s="46" t="s">
@@ -69009,7 +69024,7 @@
       </c>
     </row>
     <row r="1650" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1650" s="62" t="s">
+      <c r="A1650" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1650" s="59" t="s">
@@ -69041,7 +69056,7 @@
       </c>
     </row>
     <row r="1651" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1651" s="62" t="s">
+      <c r="A1651" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1651" s="59" t="s">
@@ -69073,7 +69088,7 @@
       </c>
     </row>
     <row r="1652" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1652" s="62" t="s">
+      <c r="A1652" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1652" s="59" t="s">
@@ -69105,7 +69120,7 @@
       </c>
     </row>
     <row r="1653" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1653" s="62" t="s">
+      <c r="A1653" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1653" s="59" t="s">
@@ -69137,7 +69152,7 @@
       </c>
     </row>
     <row r="1654" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1654" s="62" t="s">
+      <c r="A1654" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1654" s="59" t="s">
@@ -69172,7 +69187,7 @@
       </c>
     </row>
     <row r="1655" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1655" s="62" t="s">
+      <c r="A1655" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1655" s="46" t="s">
@@ -69201,7 +69216,7 @@
       </c>
     </row>
     <row r="1656" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1656" s="62" t="s">
+      <c r="A1656" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1656" s="46" t="s">
@@ -69230,7 +69245,7 @@
       </c>
     </row>
     <row r="1657" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1657" s="62" t="s">
+      <c r="A1657" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1657" s="46" t="s">
@@ -69259,7 +69274,7 @@
       </c>
     </row>
     <row r="1658" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1658" s="62" t="s">
+      <c r="A1658" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1658" s="46" t="s">
@@ -69289,7 +69304,7 @@
       <c r="V1658" s="44"/>
     </row>
     <row r="1659" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1659" s="62" t="s">
+      <c r="A1659" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1659" s="46" t="s">
@@ -69318,7 +69333,7 @@
       </c>
     </row>
     <row r="1660" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1660" s="62" t="s">
+      <c r="A1660" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1660" s="46" t="s">
@@ -69347,7 +69362,7 @@
       </c>
     </row>
     <row r="1661" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1661" s="62" t="s">
+      <c r="A1661" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1661" s="46" t="s">
@@ -69376,7 +69391,7 @@
       </c>
     </row>
     <row r="1662" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1662" s="62" t="s">
+      <c r="A1662" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1662" s="46" t="s">
@@ -69405,7 +69420,7 @@
       </c>
     </row>
     <row r="1663" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1663" s="62" t="s">
+      <c r="A1663" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1663" s="46" t="s">
@@ -69434,7 +69449,7 @@
       </c>
     </row>
     <row r="1664" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1664" s="62" t="s">
+      <c r="A1664" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1664" s="46" t="s">
@@ -69463,7 +69478,7 @@
       </c>
     </row>
     <row r="1665" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1665" s="62" t="s">
+      <c r="A1665" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1665" s="46" t="s">
@@ -69492,7 +69507,7 @@
       </c>
     </row>
     <row r="1666" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1666" s="62" t="s">
+      <c r="A1666" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1666" s="46" t="s">
@@ -69524,7 +69539,7 @@
       </c>
     </row>
     <row r="1667" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1667" s="62" t="s">
+      <c r="A1667" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1667" s="46" t="s">
@@ -69553,7 +69568,7 @@
       </c>
     </row>
     <row r="1668" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1668" s="62" t="s">
+      <c r="A1668" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1668" s="46" t="s">
@@ -69582,7 +69597,7 @@
       </c>
     </row>
     <row r="1669" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1669" s="62" t="s">
+      <c r="A1669" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1669" s="46" t="s">
@@ -69611,7 +69626,7 @@
       </c>
     </row>
     <row r="1670" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1670" s="62" t="s">
+      <c r="A1670" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1670" s="46" t="s">
@@ -69640,7 +69655,7 @@
       </c>
     </row>
     <row r="1671" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1671" s="62" t="s">
+      <c r="A1671" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1671" s="46" t="s">
@@ -69669,7 +69684,7 @@
       </c>
     </row>
     <row r="1672" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1672" s="62" t="s">
+      <c r="A1672" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1672" s="46" t="s">
@@ -69704,7 +69719,7 @@
       </c>
     </row>
     <row r="1673" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1673" s="62" t="s">
+      <c r="A1673" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1673" s="46" t="s">
@@ -69733,7 +69748,7 @@
       </c>
     </row>
     <row r="1674" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1674" s="62" t="s">
+      <c r="A1674" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1674" s="46" t="s">
@@ -69768,7 +69783,7 @@
       </c>
     </row>
     <row r="1675" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1675" s="62" t="s">
+      <c r="A1675" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1675" s="46" t="s">
@@ -69800,7 +69815,7 @@
       </c>
     </row>
     <row r="1676" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1676" s="62" t="s">
+      <c r="A1676" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1676" s="46" t="s">
@@ -69832,7 +69847,7 @@
       </c>
     </row>
     <row r="1677" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1677" s="62" t="s">
+      <c r="A1677" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1677" s="46" t="s">
@@ -69864,7 +69879,7 @@
       </c>
     </row>
     <row r="1678" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1678" s="62" t="s">
+      <c r="A1678" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1678" s="46" t="s">
@@ -69899,7 +69914,7 @@
       </c>
     </row>
     <row r="1679" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1679" s="62" t="s">
+      <c r="A1679" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1679" s="46" t="s">
@@ -69931,7 +69946,7 @@
       </c>
     </row>
     <row r="1680" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1680" s="62" t="s">
+      <c r="A1680" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1680" s="46" t="s">
@@ -69960,7 +69975,7 @@
       </c>
     </row>
     <row r="1681" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1681" s="62" t="s">
+      <c r="A1681" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1681" s="46" t="s">
@@ -69989,7 +70004,7 @@
       </c>
     </row>
     <row r="1682" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1682" s="62" t="s">
+      <c r="A1682" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1682" s="46" t="s">
@@ -70021,7 +70036,7 @@
       </c>
     </row>
     <row r="1683" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1683" s="62" t="s">
+      <c r="A1683" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1683" s="46" t="s">
@@ -70053,7 +70068,7 @@
       </c>
     </row>
     <row r="1684" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1684" s="62" t="s">
+      <c r="A1684" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1684" s="46" t="s">
@@ -70083,7 +70098,7 @@
       <c r="V1684" s="44"/>
     </row>
     <row r="1685" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1685" s="62" t="s">
+      <c r="A1685" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1685" s="46" t="s">
@@ -70112,7 +70127,7 @@
       </c>
     </row>
     <row r="1686" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1686" s="62" t="s">
+      <c r="A1686" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1686" s="46" t="s">
@@ -70141,7 +70156,7 @@
       </c>
     </row>
     <row r="1687" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1687" s="62" t="s">
+      <c r="A1687" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1687" s="46" t="s">
@@ -70170,7 +70185,7 @@
       </c>
     </row>
     <row r="1688" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1688" s="62" t="s">
+      <c r="A1688" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1688" s="46" t="s">
@@ -70200,7 +70215,7 @@
       <c r="V1688" s="44"/>
     </row>
     <row r="1689" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1689" s="62" t="s">
+      <c r="A1689" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1689" s="46" t="s">
@@ -70232,7 +70247,7 @@
       </c>
     </row>
     <row r="1690" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1690" s="62" t="s">
+      <c r="A1690" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1690" s="46" t="s">
@@ -70264,7 +70279,7 @@
       </c>
     </row>
     <row r="1691" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1691" s="62" t="s">
+      <c r="A1691" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1691" s="46" t="s">
@@ -70293,7 +70308,7 @@
       </c>
     </row>
     <row r="1692" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1692" s="62" t="s">
+      <c r="A1692" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1692" s="46" t="s">
@@ -70325,7 +70340,7 @@
       </c>
     </row>
     <row r="1693" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1693" s="62" t="s">
+      <c r="A1693" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1693" s="46" t="s">
@@ -70354,7 +70369,7 @@
       </c>
     </row>
     <row r="1694" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1694" s="62" t="s">
+      <c r="A1694" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1694" s="46" t="s">
@@ -70383,7 +70398,7 @@
       </c>
     </row>
     <row r="1695" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1695" s="62" t="s">
+      <c r="A1695" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1695" s="46" t="s">
@@ -70412,7 +70427,7 @@
       </c>
     </row>
     <row r="1696" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1696" s="62" t="s">
+      <c r="A1696" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1696" s="46" t="s">
@@ -70444,7 +70459,7 @@
       </c>
     </row>
     <row r="1697" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1697" s="62" t="s">
+      <c r="A1697" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1697" s="46" t="s">
@@ -70473,7 +70488,7 @@
       </c>
     </row>
     <row r="1698" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1698" s="62" t="s">
+      <c r="A1698" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1698" s="46" t="s">
@@ -70505,7 +70520,7 @@
       </c>
     </row>
     <row r="1699" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1699" s="62" t="s">
+      <c r="A1699" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1699" s="46" t="s">
@@ -70537,7 +70552,7 @@
       </c>
     </row>
     <row r="1700" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1700" s="62" t="s">
+      <c r="A1700" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1700" s="46" t="s">
@@ -70569,7 +70584,7 @@
       </c>
     </row>
     <row r="1701" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1701" s="62" t="s">
+      <c r="A1701" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1701" s="46" t="s">
@@ -70599,7 +70614,7 @@
       <c r="V1701" s="44"/>
     </row>
     <row r="1702" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1702" s="62" t="s">
+      <c r="A1702" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1702" s="46" t="s">
@@ -70628,7 +70643,7 @@
       </c>
     </row>
     <row r="1703" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1703" s="62" t="s">
+      <c r="A1703" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1703" s="46" t="s">
@@ -70657,7 +70672,7 @@
       </c>
     </row>
     <row r="1704" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1704" s="62" t="s">
+      <c r="A1704" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1704" s="46" t="s">
@@ -70686,7 +70701,7 @@
       </c>
     </row>
     <row r="1705" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1705" s="62" t="s">
+      <c r="A1705" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1705" s="46" t="s">
@@ -70715,7 +70730,7 @@
       </c>
     </row>
     <row r="1706" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1706" s="62" t="s">
+      <c r="A1706" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1706" s="46" t="s">
@@ -70745,7 +70760,7 @@
       <c r="V1706" s="44"/>
     </row>
     <row r="1707" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1707" s="62" t="s">
+      <c r="A1707" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1707" s="46" t="s">
@@ -70774,7 +70789,7 @@
       </c>
     </row>
     <row r="1708" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1708" s="62" t="s">
+      <c r="A1708" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1708" s="46" t="s">
@@ -70806,7 +70821,7 @@
       </c>
     </row>
     <row r="1709" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1709" s="62" t="s">
+      <c r="A1709" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1709" s="46" t="s">
@@ -70838,7 +70853,7 @@
       </c>
     </row>
     <row r="1710" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1710" s="62" t="s">
+      <c r="A1710" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1710" s="46" t="s">
@@ -70867,7 +70882,7 @@
       </c>
     </row>
     <row r="1711" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1711" s="62" t="s">
+      <c r="A1711" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1711" s="46" t="s">
@@ -70896,7 +70911,7 @@
       </c>
     </row>
     <row r="1712" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1712" s="62" t="s">
+      <c r="A1712" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1712" s="46" t="s">
@@ -70925,7 +70940,7 @@
       </c>
     </row>
     <row r="1713" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1713" s="62" t="s">
+      <c r="A1713" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1713" s="46" t="s">
@@ -70954,7 +70969,7 @@
       </c>
     </row>
     <row r="1714" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1714" s="62" t="s">
+      <c r="A1714" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1714" s="46" t="s">
@@ -70986,7 +71001,7 @@
       </c>
     </row>
     <row r="1715" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1715" s="62" t="s">
+      <c r="A1715" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1715" s="46" t="s">
@@ -71015,7 +71030,7 @@
       </c>
     </row>
     <row r="1716" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1716" s="62" t="s">
+      <c r="A1716" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1716" s="46" t="s">
@@ -71047,7 +71062,7 @@
       </c>
     </row>
     <row r="1717" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1717" s="62" t="s">
+      <c r="A1717" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1717" s="46" t="s">
@@ -71077,7 +71092,7 @@
       <c r="V1717" s="44"/>
     </row>
     <row r="1718" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1718" s="62" t="s">
+      <c r="A1718" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1718" s="46" t="s">
@@ -71106,7 +71121,7 @@
       </c>
     </row>
     <row r="1719" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1719" s="62" t="s">
+      <c r="A1719" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1719" s="46" t="s">
@@ -71136,7 +71151,7 @@
       <c r="V1719" s="44"/>
     </row>
     <row r="1720" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1720" s="62" t="s">
+      <c r="A1720" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1720" s="46" t="s">
@@ -71165,7 +71180,7 @@
       </c>
     </row>
     <row r="1721" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1721" s="62" t="s">
+      <c r="A1721" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1721" s="46" t="s">
@@ -71197,7 +71212,7 @@
       </c>
     </row>
     <row r="1722" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1722" s="62" t="s">
+      <c r="A1722" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1722" s="46" t="s">
@@ -71226,10 +71241,10 @@
       </c>
     </row>
     <row r="1723" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1723" s="62" t="s">
+      <c r="A1723" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="G1723" s="65" t="s">
+      <c r="G1723" s="64" t="s">
         <v>1502</v>
       </c>
       <c r="I1723" s="46" t="s">
@@ -71258,10 +71273,10 @@
       </c>
     </row>
     <row r="1724" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1724" s="62" t="s">
+      <c r="A1724" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="G1724" s="65" t="s">
+      <c r="G1724" s="64" t="s">
         <v>1502</v>
       </c>
       <c r="I1724" s="46" t="s">
@@ -71290,10 +71305,10 @@
       </c>
     </row>
     <row r="1725" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1725" s="62" t="s">
+      <c r="A1725" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="G1725" s="65" t="s">
+      <c r="G1725" s="64" t="s">
         <v>1502</v>
       </c>
       <c r="I1725" s="46" t="s">
@@ -71325,7 +71340,7 @@
       </c>
     </row>
     <row r="1726" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1726" s="62" t="s">
+      <c r="A1726" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1726" s="46" t="s">
@@ -71355,7 +71370,7 @@
       <c r="V1726" s="44"/>
     </row>
     <row r="1727" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1727" s="62" t="s">
+      <c r="A1727" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1727" s="46" t="s">
@@ -71384,7 +71399,7 @@
       </c>
     </row>
     <row r="1728" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1728" s="62" t="s">
+      <c r="A1728" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1728" s="46" t="s">
@@ -71413,7 +71428,7 @@
       </c>
     </row>
     <row r="1729" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1729" s="62" t="s">
+      <c r="A1729" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1729" s="46" t="s">
@@ -71442,7 +71457,7 @@
       </c>
     </row>
     <row r="1730" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1730" s="62" t="s">
+      <c r="A1730" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1730" s="46" t="s">
@@ -71477,7 +71492,7 @@
       </c>
     </row>
     <row r="1731" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1731" s="62" t="s">
+      <c r="A1731" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1731" s="46" t="s">
@@ -71509,7 +71524,7 @@
       </c>
     </row>
     <row r="1732" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1732" s="62" t="s">
+      <c r="A1732" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1732" s="46" t="s">
@@ -71538,7 +71553,7 @@
       </c>
     </row>
     <row r="1733" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1733" s="62" t="s">
+      <c r="A1733" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1733" s="46" t="s">
@@ -71570,7 +71585,7 @@
       </c>
     </row>
     <row r="1734" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1734" s="62" t="s">
+      <c r="A1734" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1734" s="59" t="s">
@@ -71602,7 +71617,7 @@
       </c>
     </row>
     <row r="1735" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1735" s="62" t="s">
+      <c r="A1735" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1735" s="59" t="s">
@@ -71629,7 +71644,7 @@
       <c r="N1735" s="44" t="s">
         <v>967</v>
       </c>
-      <c r="U1735" s="63" t="s">
+      <c r="U1735" s="62" t="s">
         <v>1497</v>
       </c>
       <c r="V1735" s="44" t="s">
@@ -71637,7 +71652,7 @@
       </c>
     </row>
     <row r="1736" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1736" s="62" t="s">
+      <c r="A1736" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1736" s="59" t="s">
@@ -71669,7 +71684,7 @@
       </c>
     </row>
     <row r="1737" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1737" s="62" t="s">
+      <c r="A1737" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1737" s="59"/>
@@ -71702,7 +71717,7 @@
       </c>
     </row>
     <row r="1738" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1738" s="62" t="s">
+      <c r="A1738" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1738" s="46" t="s">
@@ -71734,7 +71749,7 @@
       </c>
     </row>
     <row r="1739" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1739" s="62" t="s">
+      <c r="A1739" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1739" s="59" t="s">
@@ -71767,7 +71782,7 @@
       <c r="V1739" s="44"/>
     </row>
     <row r="1740" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1740" s="62" t="s">
+      <c r="A1740" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1740" s="59" t="s">
@@ -71799,7 +71814,7 @@
       </c>
     </row>
     <row r="1741" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1741" s="62" t="s">
+      <c r="A1741" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1741" s="59" t="s">
@@ -71831,7 +71846,7 @@
       </c>
     </row>
     <row r="1742" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1742" s="62" t="s">
+      <c r="A1742" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1742" s="59" t="s">
@@ -71863,7 +71878,7 @@
       </c>
     </row>
     <row r="1743" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1743" s="62" t="s">
+      <c r="A1743" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1743" s="59" t="s">
@@ -71898,7 +71913,7 @@
       </c>
     </row>
     <row r="1744" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1744" s="62" t="s">
+      <c r="A1744" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1744" s="46" t="s">
@@ -71927,7 +71942,7 @@
       </c>
     </row>
     <row r="1745" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1745" s="62" t="s">
+      <c r="A1745" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1745" s="46" t="s">
@@ -71956,7 +71971,7 @@
       </c>
     </row>
     <row r="1746" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1746" s="62" t="s">
+      <c r="A1746" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1746" s="46" t="s">
@@ -71985,7 +72000,7 @@
       </c>
     </row>
     <row r="1747" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1747" s="62" t="s">
+      <c r="A1747" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1747" s="46" t="s">
@@ -72014,7 +72029,7 @@
       </c>
     </row>
     <row r="1748" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1748" s="62" t="s">
+      <c r="A1748" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1748" s="46" t="s">
@@ -72043,7 +72058,7 @@
       </c>
     </row>
     <row r="1749" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1749" s="62" t="s">
+      <c r="A1749" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1749" s="46" t="s">
@@ -72078,7 +72093,7 @@
       </c>
     </row>
     <row r="1750" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1750" s="62" t="s">
+      <c r="A1750" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1750" s="59" t="s">
@@ -72110,7 +72125,7 @@
       </c>
     </row>
     <row r="1751" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1751" s="62" t="s">
+      <c r="A1751" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1751" s="59" t="s">
@@ -72142,7 +72157,7 @@
       </c>
     </row>
     <row r="1752" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1752" s="62" t="s">
+      <c r="A1752" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1752" s="59" t="s">
@@ -72175,7 +72190,7 @@
       <c r="V1752" s="44"/>
     </row>
     <row r="1753" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1753" s="62" t="s">
+      <c r="A1753" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1753" s="59" t="s">
@@ -72210,7 +72225,7 @@
       </c>
     </row>
     <row r="1754" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1754" s="62" t="s">
+      <c r="A1754" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1754" s="46" t="s">
@@ -72239,7 +72254,7 @@
       </c>
     </row>
     <row r="1755" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1755" s="62" t="s">
+      <c r="A1755" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1755" s="46" t="s">
@@ -72268,7 +72283,7 @@
       </c>
     </row>
     <row r="1756" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1756" s="62" t="s">
+      <c r="A1756" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1756" s="46" t="s">
@@ -72297,7 +72312,7 @@
       </c>
     </row>
     <row r="1757" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1757" s="62" t="s">
+      <c r="A1757" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1757" s="46" t="s">
@@ -72326,7 +72341,7 @@
       </c>
     </row>
     <row r="1758" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1758" s="62" t="s">
+      <c r="A1758" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1758" s="46" t="s">
@@ -72355,7 +72370,7 @@
       </c>
     </row>
     <row r="1759" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1759" s="62" t="s">
+      <c r="A1759" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1759" s="46" t="s">
@@ -72387,7 +72402,7 @@
       </c>
     </row>
     <row r="1760" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1760" s="62" t="s">
+      <c r="A1760" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1760" s="46" t="s">
@@ -72416,7 +72431,7 @@
       </c>
     </row>
     <row r="1761" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1761" s="62" t="s">
+      <c r="A1761" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1761" s="46" t="s">
@@ -72445,7 +72460,7 @@
       </c>
     </row>
     <row r="1762" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1762" s="62" t="s">
+      <c r="A1762" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1762" s="46" t="s">
@@ -72477,7 +72492,7 @@
       </c>
     </row>
     <row r="1763" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1763" s="62" t="s">
+      <c r="A1763" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1763" s="46" t="s">
@@ -72506,7 +72521,7 @@
       </c>
     </row>
     <row r="1764" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1764" s="62" t="s">
+      <c r="A1764" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1764" s="46" t="s">
@@ -72538,7 +72553,7 @@
       </c>
     </row>
     <row r="1765" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1765" s="62" t="s">
+      <c r="A1765" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1765" s="46" t="s">
@@ -72567,7 +72582,7 @@
       </c>
     </row>
     <row r="1766" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1766" s="62" t="s">
+      <c r="A1766" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1766" s="46" t="s">
@@ -72596,7 +72611,7 @@
       </c>
     </row>
     <row r="1767" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1767" s="62" t="s">
+      <c r="A1767" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1767" s="46" t="s">
@@ -72625,7 +72640,7 @@
       </c>
     </row>
     <row r="1768" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1768" s="62" t="s">
+      <c r="A1768" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1768" s="46" t="s">
@@ -72654,7 +72669,7 @@
       </c>
     </row>
     <row r="1769" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1769" s="62" t="s">
+      <c r="A1769" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1769" s="46" t="s">
@@ -72683,7 +72698,7 @@
       </c>
     </row>
     <row r="1770" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1770" s="62" t="s">
+      <c r="A1770" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1770" s="46" t="s">
@@ -72715,7 +72730,7 @@
       </c>
     </row>
     <row r="1771" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1771" s="62" t="s">
+      <c r="A1771" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1771" s="46" t="s">
@@ -72750,7 +72765,7 @@
       </c>
     </row>
     <row r="1772" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1772" s="62" t="s">
+      <c r="A1772" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1772" s="46" t="s">
@@ -72780,7 +72795,7 @@
       <c r="V1772" s="44"/>
     </row>
     <row r="1773" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1773" s="62" t="s">
+      <c r="A1773" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1773" s="46" t="s">
@@ -72809,7 +72824,7 @@
       </c>
     </row>
     <row r="1774" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1774" s="62" t="s">
+      <c r="A1774" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1774" s="46" t="s">
@@ -72838,7 +72853,7 @@
       </c>
     </row>
     <row r="1775" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1775" s="62" t="s">
+      <c r="A1775" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1775" s="46" t="s">
@@ -72867,7 +72882,7 @@
       </c>
     </row>
     <row r="1776" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1776" s="62" t="s">
+      <c r="A1776" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1776" s="46" t="s">
@@ -72896,7 +72911,7 @@
       </c>
     </row>
     <row r="1777" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1777" s="62" t="s">
+      <c r="A1777" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1777" s="46" t="s">
@@ -72925,7 +72940,7 @@
       </c>
     </row>
     <row r="1778" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1778" s="62" t="s">
+      <c r="A1778" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1778" s="46" t="s">
@@ -72954,7 +72969,7 @@
       </c>
     </row>
     <row r="1779" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1779" s="62" t="s">
+      <c r="A1779" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1779" s="46" t="s">
@@ -72983,7 +72998,7 @@
       </c>
     </row>
     <row r="1780" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1780" s="62" t="s">
+      <c r="A1780" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1780" s="46" t="s">
@@ -73012,7 +73027,7 @@
       </c>
     </row>
     <row r="1781" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1781" s="62" t="s">
+      <c r="A1781" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1781" s="46" t="s">
@@ -73041,7 +73056,7 @@
       </c>
     </row>
     <row r="1782" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1782" s="62" t="s">
+      <c r="A1782" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1782" s="46" t="s">
@@ -73070,7 +73085,7 @@
       </c>
     </row>
     <row r="1783" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1783" s="62" t="s">
+      <c r="A1783" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1783" s="46" t="s">
@@ -73102,7 +73117,7 @@
       </c>
     </row>
     <row r="1784" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1784" s="62" t="s">
+      <c r="A1784" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1784" s="46" t="s">
@@ -73131,7 +73146,7 @@
       </c>
     </row>
     <row r="1785" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1785" s="62" t="s">
+      <c r="A1785" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1785" s="46" t="s">
@@ -73160,7 +73175,7 @@
       </c>
     </row>
     <row r="1786" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1786" s="62" t="s">
+      <c r="A1786" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1786" s="46" t="s">
@@ -73189,7 +73204,7 @@
       </c>
     </row>
     <row r="1787" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1787" s="62" t="s">
+      <c r="A1787" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1787" s="46" t="s">
@@ -73221,7 +73236,7 @@
       </c>
     </row>
     <row r="1788" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1788" s="62" t="s">
+      <c r="A1788" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1788" s="46" t="s">
@@ -73250,7 +73265,7 @@
       </c>
     </row>
     <row r="1789" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1789" s="62" t="s">
+      <c r="A1789" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1789" s="46" t="s">
@@ -73282,7 +73297,7 @@
       </c>
     </row>
     <row r="1790" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1790" s="62" t="s">
+      <c r="A1790" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1790" s="46" t="s">
@@ -73311,7 +73326,7 @@
       </c>
     </row>
     <row r="1791" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1791" s="62" t="s">
+      <c r="A1791" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1791" s="46" t="s">
@@ -73343,7 +73358,7 @@
       </c>
     </row>
     <row r="1792" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1792" s="62" t="s">
+      <c r="A1792" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1792" s="46" t="s">
@@ -73375,7 +73390,7 @@
       </c>
     </row>
     <row r="1793" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1793" s="62" t="s">
+      <c r="A1793" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1793" s="46" t="s">
@@ -73404,7 +73419,7 @@
       </c>
     </row>
     <row r="1794" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1794" s="62" t="s">
+      <c r="A1794" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1794" s="46" t="s">
@@ -73433,7 +73448,7 @@
       </c>
     </row>
     <row r="1795" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1795" s="62" t="s">
+      <c r="A1795" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1795" s="46" t="s">
@@ -73462,7 +73477,7 @@
       </c>
     </row>
     <row r="1796" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1796" s="62" t="s">
+      <c r="A1796" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1796" s="46" t="s">
@@ -73491,7 +73506,7 @@
       </c>
     </row>
     <row r="1797" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1797" s="62" t="s">
+      <c r="A1797" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1797" s="46" t="s">
@@ -73520,7 +73535,7 @@
       </c>
     </row>
     <row r="1798" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1798" s="62" t="s">
+      <c r="A1798" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1798" s="46" t="s">
@@ -73549,7 +73564,7 @@
       </c>
     </row>
     <row r="1799" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1799" s="62" t="s">
+      <c r="A1799" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1799" s="46" t="s">
@@ -73578,7 +73593,7 @@
       </c>
     </row>
     <row r="1800" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1800" s="62" t="s">
+      <c r="A1800" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1800" s="46" t="s">
@@ -73607,7 +73622,7 @@
       </c>
     </row>
     <row r="1801" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1801" s="62" t="s">
+      <c r="A1801" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1801" s="46" t="s">
@@ -73639,7 +73654,7 @@
       </c>
     </row>
     <row r="1802" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1802" s="62" t="s">
+      <c r="A1802" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1802" s="46" t="s">
@@ -73668,7 +73683,7 @@
       </c>
     </row>
     <row r="1803" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1803" s="62" t="s">
+      <c r="A1803" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1803" s="46" t="s">
@@ -73697,7 +73712,7 @@
       </c>
     </row>
     <row r="1804" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1804" s="62" t="s">
+      <c r="A1804" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1804" s="46" t="s">
@@ -73727,7 +73742,7 @@
       <c r="V1804" s="44"/>
     </row>
     <row r="1805" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1805" s="62" t="s">
+      <c r="A1805" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1805" s="46" t="s">
@@ -73756,7 +73771,7 @@
       </c>
     </row>
     <row r="1806" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1806" s="62" t="s">
+      <c r="A1806" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1806" s="46" t="s">
@@ -73785,7 +73800,7 @@
       </c>
     </row>
     <row r="1807" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1807" s="62" t="s">
+      <c r="A1807" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1807" s="46" t="s">
@@ -73815,7 +73830,7 @@
       <c r="V1807" s="44"/>
     </row>
     <row r="1808" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1808" s="62" t="s">
+      <c r="A1808" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1808" s="46" t="s">
@@ -73844,7 +73859,7 @@
       </c>
     </row>
     <row r="1809" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1809" s="62" t="s">
+      <c r="A1809" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1809" s="46" t="s">
@@ -73873,7 +73888,7 @@
       </c>
     </row>
     <row r="1810" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1810" s="62" t="s">
+      <c r="A1810" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1810" s="46" t="s">
@@ -73905,7 +73920,7 @@
       </c>
     </row>
     <row r="1811" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1811" s="62" t="s">
+      <c r="A1811" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1811" s="46" t="s">
@@ -73937,7 +73952,7 @@
       </c>
     </row>
     <row r="1812" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1812" s="62" t="s">
+      <c r="A1812" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1812" s="46" t="s">
@@ -73969,7 +73984,7 @@
       </c>
     </row>
     <row r="1813" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1813" s="62" t="s">
+      <c r="A1813" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1813" s="46" t="s">
@@ -74001,7 +74016,7 @@
       </c>
     </row>
     <row r="1814" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1814" s="62" t="s">
+      <c r="A1814" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1814" s="46" t="s">
@@ -74030,7 +74045,7 @@
       </c>
     </row>
     <row r="1815" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1815" s="62" t="s">
+      <c r="A1815" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1815" s="46" t="s">
@@ -74059,7 +74074,7 @@
       </c>
     </row>
     <row r="1816" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1816" s="62" t="s">
+      <c r="A1816" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1816" s="46" t="s">
@@ -74091,7 +74106,7 @@
       </c>
     </row>
     <row r="1817" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1817" s="62" t="s">
+      <c r="A1817" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1817" s="46" t="s">
@@ -74123,7 +74138,7 @@
       </c>
     </row>
     <row r="1818" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1818" s="62" t="s">
+      <c r="A1818" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1818" s="46" t="s">
@@ -74158,7 +74173,7 @@
       </c>
     </row>
     <row r="1819" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1819" s="62" t="s">
+      <c r="A1819" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1819" s="46" t="s">
@@ -74187,7 +74202,7 @@
       </c>
     </row>
     <row r="1820" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1820" s="62" t="s">
+      <c r="A1820" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1820" s="46" t="s">
@@ -74216,7 +74231,7 @@
       </c>
     </row>
     <row r="1821" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1821" s="62" t="s">
+      <c r="A1821" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1821" s="46" t="s">
@@ -74245,7 +74260,7 @@
       </c>
     </row>
     <row r="1822" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1822" s="62" t="s">
+      <c r="A1822" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1822" s="46" t="s">
@@ -74274,7 +74289,7 @@
       </c>
     </row>
     <row r="1823" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1823" s="62" t="s">
+      <c r="A1823" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1823" s="46" t="s">
@@ -74303,7 +74318,7 @@
       </c>
     </row>
     <row r="1824" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1824" s="62" t="s">
+      <c r="A1824" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1824" s="46" t="s">
@@ -74332,7 +74347,7 @@
       </c>
     </row>
     <row r="1825" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1825" s="62" t="s">
+      <c r="A1825" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1825" s="46" t="s">
@@ -74367,7 +74382,7 @@
       </c>
     </row>
     <row r="1826" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1826" s="62" t="s">
+      <c r="A1826" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1826" s="46" t="s">
@@ -74396,7 +74411,7 @@
       </c>
     </row>
     <row r="1827" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1827" s="62" t="s">
+      <c r="A1827" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1827" s="46" t="s">
@@ -74425,7 +74440,7 @@
       </c>
     </row>
     <row r="1828" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1828" s="62" t="s">
+      <c r="A1828" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1828" s="46" t="s">
@@ -74457,7 +74472,7 @@
       </c>
     </row>
     <row r="1829" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1829" s="62" t="s">
+      <c r="A1829" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1829" s="46" t="s">
@@ -74489,7 +74504,7 @@
       </c>
     </row>
     <row r="1830" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1830" s="62" t="s">
+      <c r="A1830" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1830" s="59" t="s">
@@ -74521,7 +74536,7 @@
       </c>
     </row>
     <row r="1831" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1831" s="62" t="s">
+      <c r="A1831" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1831" s="59" t="s">
@@ -74553,10 +74568,10 @@
       </c>
     </row>
     <row r="1832" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1832" s="62" t="s">
+      <c r="A1832" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="E1832" s="65" t="s">
+      <c r="E1832" s="64" t="s">
         <v>1503</v>
       </c>
       <c r="H1832" s="59" t="s">
@@ -74588,10 +74603,10 @@
       </c>
     </row>
     <row r="1833" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1833" s="62" t="s">
+      <c r="A1833" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="E1833" s="65" t="s">
+      <c r="E1833" s="64" t="s">
         <v>1503</v>
       </c>
       <c r="H1833" s="59" t="s">
@@ -74623,7 +74638,7 @@
       </c>
     </row>
     <row r="1834" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1834" s="62" t="s">
+      <c r="A1834" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1834" s="59" t="s">
@@ -74655,7 +74670,7 @@
       </c>
     </row>
     <row r="1835" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1835" s="62" t="s">
+      <c r="A1835" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="H1835" s="59" t="s">
@@ -74687,7 +74702,7 @@
       </c>
     </row>
     <row r="1836" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1836" s="62" t="s">
+      <c r="A1836" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1836" s="46" t="s">
@@ -74716,7 +74731,7 @@
       </c>
     </row>
     <row r="1837" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1837" s="62" t="s">
+      <c r="A1837" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1837" s="46" t="s">
@@ -74746,7 +74761,7 @@
       <c r="V1837" s="44"/>
     </row>
     <row r="1838" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1838" s="62" t="s">
+      <c r="A1838" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1838" s="46" t="s">
@@ -74775,7 +74790,7 @@
       </c>
     </row>
     <row r="1839" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1839" s="62" t="s">
+      <c r="A1839" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1839" s="46" t="s">
@@ -74804,7 +74819,7 @@
       </c>
     </row>
     <row r="1840" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1840" s="62" t="s">
+      <c r="A1840" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1840" s="46" t="s">
@@ -74836,7 +74851,7 @@
       </c>
     </row>
     <row r="1841" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1841" s="62" t="s">
+      <c r="A1841" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1841" s="46" t="s">
@@ -74865,7 +74880,7 @@
       </c>
     </row>
     <row r="1842" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1842" s="62" t="s">
+      <c r="A1842" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1842" s="46" t="s">
@@ -74894,7 +74909,7 @@
       </c>
     </row>
     <row r="1843" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1843" s="62" t="s">
+      <c r="A1843" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1843" s="46" t="s">
@@ -74926,7 +74941,7 @@
       </c>
     </row>
     <row r="1844" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1844" s="62" t="s">
+      <c r="A1844" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1844" s="46" t="s">
@@ -74955,7 +74970,7 @@
       </c>
     </row>
     <row r="1845" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1845" s="62" t="s">
+      <c r="A1845" s="61" t="s">
         <v>1483</v>
       </c>
       <c r="I1845" s="46" t="s">

</xml_diff>